<commit_message>
create Image processing app
</commit_message>
<xml_diff>
--- a/Project_German_Learning_Tool/German_vocab_new.xlsx
+++ b/Project_German_Learning_Tool/German_vocab_new.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" fullCalcOnLoad="true"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Entscheidung</t>
   </si>
@@ -36,156 +36,6 @@
   </si>
   <si>
     <t>to choose</t>
-  </si>
-  <si>
-    <t>Fähigkeiten</t>
-  </si>
-  <si>
-    <t>Entspannen</t>
-  </si>
-  <si>
-    <t>Reinlich</t>
-  </si>
-  <si>
-    <t>Aufmerksam</t>
-  </si>
-  <si>
-    <t>Erzieher</t>
-  </si>
-  <si>
-    <t>Fertig</t>
-  </si>
-  <si>
-    <t>Ausbildung</t>
-  </si>
-  <si>
-    <t>Verschieden</t>
-  </si>
-  <si>
-    <t>Erledigen</t>
-  </si>
-  <si>
-    <t>Bedeuten</t>
-  </si>
-  <si>
-    <t>entschließen</t>
-  </si>
-  <si>
-    <t>betriebsklima</t>
-  </si>
-  <si>
-    <t>bewerbung</t>
-  </si>
-  <si>
-    <t>geschieden</t>
-  </si>
-  <si>
-    <t>gefallen</t>
-  </si>
-  <si>
-    <t>skills</t>
-  </si>
-  <si>
-    <t>Relax</t>
-  </si>
-  <si>
-    <t>Clean</t>
-  </si>
-  <si>
-    <t>Attentive</t>
-  </si>
-  <si>
-    <t>Educator</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>training</t>
-  </si>
-  <si>
-    <t>different</t>
-  </si>
-  <si>
-    <t>to handle</t>
-  </si>
-  <si>
-    <t>to mean</t>
-  </si>
-  <si>
-    <t>to decide</t>
-  </si>
-  <si>
-    <t>atmosphere</t>
-  </si>
-  <si>
-    <t>application</t>
-  </si>
-  <si>
-    <t>divorced</t>
-  </si>
-  <si>
-    <t>to like</t>
-  </si>
-  <si>
-    <t>schälen</t>
-  </si>
-  <si>
-    <t>to peel</t>
-  </si>
-  <si>
-    <t>verstehen</t>
-  </si>
-  <si>
-    <t>to understand</t>
-  </si>
-  <si>
-    <t>vorstellen</t>
-  </si>
-  <si>
-    <t>to present</t>
-  </si>
-  <si>
-    <t>geschichte</t>
-  </si>
-  <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>inhalt</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>gefühl</t>
-  </si>
-  <si>
-    <t>feeling</t>
-  </si>
-  <si>
-    <t>äußern</t>
-  </si>
-  <si>
-    <t>to express</t>
-  </si>
-  <si>
-    <t>vermutung</t>
-  </si>
-  <si>
-    <t>assumption</t>
-  </si>
-  <si>
-    <t>probieren</t>
-  </si>
-  <si>
-    <t>to taste</t>
-  </si>
-  <si>
-    <t>durst</t>
-  </si>
-  <si>
-    <t>thirst</t>
   </si>
   <si>
     <t>Entspannen</t>
@@ -353,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -361,14 +211,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,20 +497,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.046875" customWidth="true"/>
-    <col min="2" max="2" width="12.48828125" customWidth="true"/>
-    <col min="3" max="3" width="3.15625" customWidth="true"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -684,274 +532,269 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
-      <c r="A3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.3">
-      <c r="A4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.3">
-      <c r="A5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="0">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
-      <c r="A6" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="0">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
-      <c r="A7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="0">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
-      <c r="A8" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="0">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
-      <c r="A9" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="0">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
-      <c r="A10" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.3">
-      <c r="A11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="0">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
-      <c r="A12" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="0">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
-      <c r="A14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="0">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="0">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
-      <c r="A16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="0">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
-      <c r="A17" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="0">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
         <v>1</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" x14ac:dyDescent="0.3">
-      <c r="A19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" x14ac:dyDescent="0.3">
-      <c r="A20" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" x14ac:dyDescent="0.3">
-      <c r="A21" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" x14ac:dyDescent="0.3">
-      <c r="A22" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" x14ac:dyDescent="0.3">
-      <c r="A23" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="0">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
-      <c r="A25" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" x14ac:dyDescent="0.3">
-      <c r="A26" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" x14ac:dyDescent="0.3">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>